<commit_message>
Final change ready for exam
</commit_message>
<xml_diff>
--- a/TestP5-LucasG.xlsx
+++ b/TestP5-LucasG.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="36">
   <si>
     <t>Fonctionnalité</t>
   </si>
@@ -25,7 +25,7 @@
     <t>Résultat final</t>
   </si>
   <si>
-    <t>Page d'acceuil affichant chaques canapés disponible en stock
+    <t>Page d'accueil affichant chaque canapé disponible en stock
 L'affichage doit être dynamique et afficher les données à partir de l'API.
 Les canapés doivent être cliquables.</t>
   </si>
@@ -33,63 +33,62 @@
     <t>&gt;</t>
   </si>
   <si>
-    <t>Ouvrir la page d'acceuil du site,
-verifier que tout les produits
+    <t>Ouvrir la page d'accueil du site;
+Vérifier que tous les produits
 sont affichés avec les bonnes données.
-Verifier que les produits sont cliquables</t>
+Vérifier que les produits sont cliquables</t>
   </si>
   <si>
     <t>Les produits sont bien affichés
- et les données sont corrects</t>
+ et les données sont correctes</t>
   </si>
   <si>
     <t>OK</t>
   </si>
   <si>
     <t>Page produit qui affiche le produit cliqué par l'utilisateur
-depuis la page d'acceuil.
+depuis la page d'accueil.
 L'affichage doit se faire dynamiquement si lors du
  clique de l'utilisateur le prix ou les couleurs disponibles changent.</t>
   </si>
   <si>
-    <t xml:space="preserve">Cliquer sur un produit à partir de la page d'acceuil,
+    <t>Cliquer sur un produit à partir de la page d'accueil;
 cela doit nous rediriger vers une nouvelle page
-avec les informations du produits cliqué préalablement
-</t>
-  </si>
-  <si>
-    <t>Le produits est bien affiché
- et les données sont corrects</t>
+avec les informations du produit cliqué précedement</t>
+  </si>
+  <si>
+    <t>Le produit est bien affiché
+ et les données sont correctes</t>
   </si>
   <si>
     <t>La page produit qui affiche le produit cliqué par l'utilisateur
-depuis la page d'acceuil, l'utilisateur doit pouvoir selectionner une quantité 
+depuis la page d'accueil, l'utilisateur doit pouvoir sélectionner une quantité 
 ainsi qu'une couleur et pouvoir ajouter l'article 
 dans son panier avec la bonne couleur et la bonne quantité.</t>
   </si>
   <si>
-    <t>Ajouter une quantité et selectionner une couleur
+    <t>Ajouter une quantité et sélectionner une couleur
 sur l'article affiché à l'écran et cliquer sur le bouton
 "Ajouter au panier". Regarder sur la page panier si notre
 article y est bien avec la bonne quantité et couleur.</t>
   </si>
   <si>
-    <t>L'utilisateur à pu selectionner une quantitée
+    <t>L'utilisateur à put sélectionner une quantité
  ainsi qu'une couleur et ajouter l'article 
-a son panier. L'article
-est bien présent sur la page Panier.</t>
+À son panier. L'article
+est bien présent sur la page panier.</t>
   </si>
   <si>
     <t>Une page panier qui contient les articles que l'utilisateur
- à selectionné</t>
-  </si>
-  <si>
-    <t>Cliquer sur la page panier et verifier que
+ à sélectionné</t>
+  </si>
+  <si>
+    <t>Cliquer sur la page panier et vérifier que
  les produits sont bien présents</t>
   </si>
   <si>
-    <t>Les produits sont présent sur la page panier
-avec les bonne quantitée et couleurs.</t>
+    <t>Les produits sont présents sur la page panier
+Avec les bonnes quantités et couleurs.</t>
   </si>
   <si>
     <t>Possibilité de changer la quantité d'un article dans le panier</t>
@@ -115,34 +114,44 @@
  global se mettent bien à jour</t>
   </si>
   <si>
-    <t>Affichage de la quantité et du prix total dynamique sur la page panier</t>
+    <t>Affichage de la quantité dynamique sur la page panier</t>
+  </si>
+  <si>
+    <t>Cliquer sur la page panier et supprimer ou modifier
+ la quantité d'un article et vérifier que la quantité totale 
+se met bien à jour sans rafraichir la page</t>
+  </si>
+  <si>
+    <t>La quantité global se met bien à jour</t>
+  </si>
+  <si>
+    <t>Affichage du prix total dynamique sur la page panier</t>
   </si>
   <si>
     <t>Cliquer sur la page panier et supprimer
  un article et/ou modifier la quantité d'un article
-et verifier que le prix total et la quantité total 
-ce mettent bien à jour sans rafraichir la page</t>
-  </si>
-  <si>
-    <t>le prix global et la quantité
- global se mettent bien à jour</t>
-  </si>
-  <si>
-    <t>Obliger l'utilisateur à correctement remplir le formulaire dans la page panier
-(Données correct et bien formatées)</t>
-  </si>
-  <si>
-    <t>Cliquer sur la page panier et essayer de remplire
-le formulaire avec des données éronées
- (caractéres spéciaux pour les champs
-nom, prénom -
- ne pas ajouter "@" pour l'adresse email etc)</t>
+et vérifier que le prix total se met bien à jour sans rafraichir la page</t>
+  </si>
+  <si>
+    <t>Le prix
+ global se met bien à jour</t>
+  </si>
+  <si>
+    <t>Verifier que les données du formulaire sur la page panier
+soient correctes (Données correctes et bien formatées)</t>
+  </si>
+  <si>
+    <t>Cliquer sur la page panier et essayer de remplir
+le formulaire avec des données erronées
+ (Caractères spéciaux pour les champs
+nom, prénom ;
+ ne pas ajouter "@" pour l'adresse email etc.)</t>
   </si>
   <si>
     <t>Des messages d'erreur apparaissent pour
  indiqué à l'utilisateur que les données
  dans le formulaire ne sont pas conformes
- aux restrictions en vigeur. Cela empeche l'utilisateur
+ aux restrictions en vigueur. Cela empêche l'utilisateur
  d'envoyer la commande
 si les champs ne sont pas
  correctement remplis.</t>
@@ -216,7 +225,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border/>
     <border>
       <left style="thin">
@@ -260,11 +269,21 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -294,6 +313,8 @@
     <xf borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
+    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -504,6 +525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -852,92 +874,155 @@
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="4"/>
-      <c r="E24" s="5" t="s">
-        <v>5</v>
-      </c>
       <c r="F24" s="6" t="s">
         <v>28</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="4"/>
-      <c r="I24" s="5" t="s">
-        <v>5</v>
-      </c>
       <c r="J24" s="6" t="s">
         <v>29</v>
       </c>
       <c r="K24" s="3"/>
       <c r="L24" s="4"/>
-      <c r="M24" s="5" t="s">
-        <v>5</v>
-      </c>
       <c r="N24" s="12" t="s">
         <v>8</v>
       </c>
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
     </row>
-    <row r="25" ht="83.25" customHeight="1">
-      <c r="B25" s="8"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="10"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="10"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="10"/>
-      <c r="N25" s="8"/>
-      <c r="O25" s="9"/>
-      <c r="P25" s="9"/>
+    <row r="25">
+      <c r="B25" s="13"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="13"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J25" s="13"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N25" s="13"/>
+    </row>
+    <row r="26">
+      <c r="B26" s="13"/>
+      <c r="D26" s="14"/>
+      <c r="F26" s="13"/>
+      <c r="H26" s="14"/>
+      <c r="J26" s="13"/>
+      <c r="L26" s="14"/>
+      <c r="N26" s="13"/>
     </row>
     <row r="27">
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="8"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="10"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="10"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="10"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="9"/>
+    </row>
+    <row r="30">
+      <c r="B30" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F27" s="6" t="s">
+      <c r="C30" s="3"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F30" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G27" s="3"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="J27" s="6" t="s">
+      <c r="G30" s="3"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J30" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="K27" s="3"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="N27" s="12" t="s">
+      <c r="K30" s="3"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N30" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="O27" s="3"/>
-      <c r="P27" s="3"/>
-    </row>
-    <row r="28" ht="36.75" customHeight="1">
-      <c r="B28" s="8"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="10"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="10"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="10"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="9"/>
-      <c r="P28" s="9"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+    </row>
+    <row r="31" ht="83.25" customHeight="1">
+      <c r="B31" s="8"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="10"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="10"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="10"/>
+      <c r="N31" s="8"/>
+      <c r="O31" s="9"/>
+      <c r="P31" s="9"/>
+    </row>
+    <row r="33">
+      <c r="B33" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G33" s="3"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K33" s="3"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N33" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+    </row>
+    <row r="34" ht="36.75" customHeight="1">
+      <c r="B34" s="8"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="10"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="10"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="10"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="9"/>
+      <c r="P34" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="67">
+  <mergeCells count="74">
     <mergeCell ref="B15:D16"/>
     <mergeCell ref="E15:E16"/>
     <mergeCell ref="F15:H16"/>
@@ -959,13 +1044,26 @@
     <mergeCell ref="J21:L22"/>
     <mergeCell ref="M21:M22"/>
     <mergeCell ref="N21:P22"/>
-    <mergeCell ref="B24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="F24:H25"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="J24:L25"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="N24:P25"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F24:H27"/>
+    <mergeCell ref="J24:L27"/>
+    <mergeCell ref="N24:P27"/>
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="I25:I26"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="N33:P34"/>
+    <mergeCell ref="M33:M34"/>
+    <mergeCell ref="J33:L34"/>
+    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="F33:H34"/>
+    <mergeCell ref="B33:D34"/>
+    <mergeCell ref="N30:P31"/>
+    <mergeCell ref="M30:M31"/>
+    <mergeCell ref="J30:L31"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="F30:H31"/>
+    <mergeCell ref="B30:D31"/>
+    <mergeCell ref="B24:D27"/>
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="J3:L4"/>
     <mergeCell ref="M3:M4"/>
@@ -998,14 +1096,11 @@
     <mergeCell ref="J12:L13"/>
     <mergeCell ref="M12:M13"/>
     <mergeCell ref="N12:P13"/>
-    <mergeCell ref="B27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:H28"/>
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="J27:L28"/>
-    <mergeCell ref="M27:M28"/>
-    <mergeCell ref="N27:P28"/>
+    <mergeCell ref="E25:E26"/>
   </mergeCells>
+  <printOptions gridLines="1" horizontalCentered="1"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>